<commit_message>
cleanup process to get to a food group lookup process.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="880" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$62</definedName>
   </definedNames>
-  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="154">
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>cbeef</t>
   </si>
   <si>
@@ -260,18 +257,6 @@
     <t>sugar and sweeteners</t>
   </si>
   <si>
-    <t>Food groups</t>
-  </si>
-  <si>
-    <t>Food group assignment</t>
-  </si>
-  <si>
-    <t>food group code</t>
-  </si>
-  <si>
-    <t>Food group codes</t>
-  </si>
-  <si>
     <t>beverages</t>
   </si>
   <si>
@@ -287,9 +272,6 @@
     <t>IMPACT_code</t>
   </si>
   <si>
-    <t>staple category</t>
-  </si>
-  <si>
     <t>nonstaple</t>
   </si>
   <si>
@@ -374,9 +356,6 @@
     <t>Aquatic plants</t>
   </si>
   <si>
-    <t>staple code</t>
-  </si>
-  <si>
     <t>alcohol</t>
   </si>
   <si>
@@ -492,6 +471,27 @@
   </si>
   <si>
     <t>Marine fish, other</t>
+  </si>
+  <si>
+    <t>food_groups</t>
+  </si>
+  <si>
+    <t>food_group_codes</t>
+  </si>
+  <si>
+    <t>food_group_assignment</t>
+  </si>
+  <si>
+    <t>food_group_code</t>
+  </si>
+  <si>
+    <t>staple_category</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>staple_code</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1048,1311 +1048,1311 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="6" t="str">
-        <f>VLOOKUP(C2,F$2:G$15,2)</f>
+        <f t="shared" ref="D2:D16" si="0">VLOOKUP(C2,F$2:G$15,2)</f>
         <v>meats</v>
       </c>
       <c r="E2" s="6" t="str">
-        <f>VLOOKUP(D2,G$2:H$15,2)</f>
+        <f t="shared" ref="E2:E16" si="1">VLOOKUP(D2,G$2:H$15,2)</f>
         <v>nonstaple</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="6" t="str">
-        <f>VLOOKUP(C3,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>vegetables</v>
       </c>
       <c r="E3" s="6" t="str">
-        <f>VLOOKUP(D3,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="D4" s="6" t="str">
-        <f>VLOOKUP(C4,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>alcohol</v>
       </c>
       <c r="E4" s="6" t="str">
-        <f>VLOOKUP(D4,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="6" t="str">
-        <f>VLOOKUP(C5,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E5" s="6" t="str">
-        <f>VLOOKUP(D5,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="6" t="str">
-        <f>VLOOKUP(C6,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E6" s="6" t="str">
-        <f>VLOOKUP(D6,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="6" t="str">
-        <f>VLOOKUP(C7,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>oils</v>
       </c>
       <c r="E7" s="6" t="str">
-        <f>VLOOKUP(D7,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="6" t="str">
-        <f>VLOOKUP(C8,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E8" s="6" t="str">
-        <f>VLOOKUP(D8,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>fish</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>nonstaple</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="6" t="str">
-        <f>VLOOKUP(C9,F$2:G$15,2)</f>
-        <v>fish</v>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f>VLOOKUP(D9,G$2:H$15,2)</f>
-        <v>nonstaple</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="G9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="6" t="str">
-        <f>VLOOKUP(C10,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E10" s="6" t="str">
-        <f>VLOOKUP(D10,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="6" t="str">
-        <f>VLOOKUP(C11,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E11" s="6" t="str">
-        <f>VLOOKUP(D11,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="6" t="str">
-        <f>VLOOKUP(C12,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E12" s="6" t="str">
-        <f>VLOOKUP(D12,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6" t="str">
-        <f>VLOOKUP(C13,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f>VLOOKUP(D13,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D14" s="6" t="str">
-        <f>VLOOKUP(C14,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>alcohol</v>
       </c>
       <c r="E14" s="6" t="str">
-        <f>VLOOKUP(D14,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="6" t="str">
-        <f>VLOOKUP(C15,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>fish</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f>VLOOKUP(D15,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D16" s="6" t="str">
-        <f>VLOOKUP(C16,F$2:G$15,2)</f>
+        <f t="shared" si="0"/>
         <v>alcohol</v>
       </c>
       <c r="E16" s="6" t="str">
-        <f>VLOOKUP(D16,G$2:H$15,2)</f>
+        <f t="shared" si="1"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="C17" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" s="6" t="str">
-        <f>VLOOKUP(D17,G$2:H$15,2)</f>
+        <f t="shared" ref="E17:E62" si="2">VLOOKUP(D17,G$2:H$15,2)</f>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="C18" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="6" t="str">
-        <f>VLOOKUP(C18,F$2:G$15,2)</f>
+        <f t="shared" ref="D18:D62" si="3">VLOOKUP(C18,F$2:G$15,2)</f>
         <v>cereals</v>
       </c>
       <c r="E18" s="6" t="str">
-        <f>VLOOKUP(D18,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="6" t="str">
-        <f>VLOOKUP(C19,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E19" s="6" t="str">
-        <f>VLOOKUP(D19,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="6" t="str">
-        <f>VLOOKUP(C20,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>meats</v>
       </c>
       <c r="E20" s="6" t="str">
-        <f>VLOOKUP(D20,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>61</v>
-      </c>
       <c r="C21" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D21" s="6" t="str">
-        <f>VLOOKUP(C21,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>beverages</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f>VLOOKUP(D21,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>21</v>
-      </c>
       <c r="C22" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D22" s="6" t="str">
-        <f>VLOOKUP(C22,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>rootsNPlaintain</v>
       </c>
       <c r="E22" s="6" t="str">
-        <f>VLOOKUP(D22,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="6" t="str">
-        <f>VLOOKUP(C23,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E23" s="6" t="str">
-        <f>VLOOKUP(D23,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="C24" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D24" s="6" t="str">
-        <f>VLOOKUP(C24,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f>VLOOKUP(D24,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>31</v>
-      </c>
       <c r="C25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="6" t="str">
-        <f>VLOOKUP(C25,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E25" s="6" t="str">
-        <f>VLOOKUP(D25,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>6</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" s="6" t="str">
-        <f>VLOOKUP(C26,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>eggs</v>
       </c>
       <c r="E26" s="6" t="str">
-        <f>VLOOKUP(D26,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="6" t="str">
-        <f>VLOOKUP(C27,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E27" s="6" t="str">
-        <f>VLOOKUP(D27,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D28" s="6" t="str">
-        <f>VLOOKUP(C28,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E28" s="6" t="str">
-        <f>VLOOKUP(D28,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" s="6" t="str">
-        <f>VLOOKUP(C29,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>meats</v>
       </c>
       <c r="E29" s="6" t="str">
-        <f>VLOOKUP(D29,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="C30" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="6" t="str">
-        <f>VLOOKUP(C30,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E30" s="6" t="str">
-        <f>VLOOKUP(D30,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>11</v>
-      </c>
       <c r="C31" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="6" t="str">
-        <f>VLOOKUP(C31,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>cereals</v>
       </c>
       <c r="E31" s="6" t="str">
-        <f>VLOOKUP(D31,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="6" t="str">
-        <f>VLOOKUP(C32,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>dairy</v>
       </c>
       <c r="E32" s="6" t="str">
-        <f>VLOOKUP(D32,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="6" t="str">
-        <f>VLOOKUP(C33,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>cereals</v>
       </c>
       <c r="E33" s="6" t="str">
-        <f>VLOOKUP(D33,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" s="6" t="str">
-        <f>VLOOKUP(C34,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>cereals</v>
       </c>
       <c r="E34" s="6" t="str">
-        <f>VLOOKUP(D34,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" s="6" t="str">
-        <f>VLOOKUP(C35,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E35" s="6" t="str">
-        <f>VLOOKUP(D35,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D36" s="6" t="str">
-        <f>VLOOKUP(C36,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>rootsNPlaintain</v>
       </c>
       <c r="E36" s="6" t="str">
-        <f>VLOOKUP(D36,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D37" s="6" t="str">
-        <f>VLOOKUP(C37,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E37" s="6" t="str">
-        <f>VLOOKUP(D37,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D38" s="6" t="str">
-        <f>VLOOKUP(C38,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E38" s="6" t="str">
-        <f>VLOOKUP(D38,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D39" s="6" t="str">
-        <f>VLOOKUP(C39,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E39" s="6" t="str">
-        <f>VLOOKUP(D39,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="C40" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D40" s="6" t="str">
-        <f>VLOOKUP(C40,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>rootsNPlaintain</v>
       </c>
       <c r="E40" s="6" t="str">
-        <f>VLOOKUP(D40,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="6" t="str">
-        <f>VLOOKUP(C41,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E41" s="6" t="str">
-        <f>VLOOKUP(D41,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D42" s="6" t="str">
-        <f>VLOOKUP(C42,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>meats</v>
       </c>
       <c r="E42" s="6" t="str">
-        <f>VLOOKUP(D42,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D43" s="6" t="str">
-        <f>VLOOKUP(C43,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>rootsNPlaintain</v>
       </c>
       <c r="E43" s="6" t="str">
-        <f>VLOOKUP(D43,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" s="6" t="str">
-        <f>VLOOKUP(C44,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>meats</v>
       </c>
       <c r="E44" s="6" t="str">
-        <f>VLOOKUP(D44,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D45" s="6" t="str">
-        <f>VLOOKUP(C45,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>cereals</v>
       </c>
       <c r="E45" s="6" t="str">
-        <f>VLOOKUP(D45,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="6" t="str">
-        <f>VLOOKUP(C46,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E46" s="6" t="str">
-        <f>VLOOKUP(D46,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="C47" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D47" s="6" t="str">
-        <f>VLOOKUP(C47,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E47" s="6" t="str">
-        <f>VLOOKUP(D47,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D48" s="6" t="str">
-        <f>VLOOKUP(C48,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E48" s="6" t="str">
-        <f>VLOOKUP(D48,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D49" s="6" t="str">
-        <f>VLOOKUP(C49,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E49" s="6" t="str">
-        <f>VLOOKUP(D49,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D50" s="6" t="str">
-        <f>VLOOKUP(C50,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E50" s="6" t="str">
-        <f>VLOOKUP(D50,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="C51" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D51" s="6" t="str">
-        <f>VLOOKUP(C51,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>cereals</v>
       </c>
       <c r="E51" s="6" t="str">
-        <f>VLOOKUP(D51,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D52" s="6" t="str">
-        <f>VLOOKUP(C52,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E52" s="6" t="str">
-        <f>VLOOKUP(D52,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D53" s="6" t="str">
-        <f>VLOOKUP(C53,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>fruits</v>
       </c>
       <c r="E53" s="6" t="str">
-        <f>VLOOKUP(D53,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54" s="6" t="str">
-        <f>VLOOKUP(C54,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>sweeteners</v>
       </c>
       <c r="E54" s="6" t="str">
-        <f>VLOOKUP(D54,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D55" s="6" t="str">
-        <f>VLOOKUP(C55,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>rootsNPlaintain</v>
       </c>
       <c r="E55" s="6" t="str">
-        <f>VLOOKUP(D55,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="C56" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D56" s="6" t="str">
-        <f>VLOOKUP(C56,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>beverages</v>
       </c>
       <c r="E56" s="6" t="str">
-        <f>VLOOKUP(D56,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D57" s="6" t="str">
-        <f>VLOOKUP(C57,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>fruits</v>
       </c>
       <c r="E57" s="6" t="str">
-        <f>VLOOKUP(D57,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D58" s="6" t="str">
-        <f>VLOOKUP(C58,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>nutsNseeds</v>
       </c>
       <c r="E58" s="6" t="str">
-        <f>VLOOKUP(D58,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" s="6" t="str">
-        <f>VLOOKUP(C59,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>oils</v>
       </c>
       <c r="E59" s="6" t="str">
-        <f>VLOOKUP(D59,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="C60" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" s="6" t="str">
-        <f>VLOOKUP(C60,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>vegetables</v>
       </c>
       <c r="E60" s="6" t="str">
-        <f>VLOOKUP(D60,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>nonstaple</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C61" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" s="6" t="str">
-        <f>VLOOKUP(C61,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>cereals</v>
       </c>
       <c r="E61" s="6" t="str">
-        <f>VLOOKUP(D61,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="C62" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" s="6" t="str">
-        <f>VLOOKUP(C62,F$2:G$15,2)</f>
+        <f t="shared" si="3"/>
         <v>pulses</v>
       </c>
       <c r="E62" s="6" t="str">
-        <f>VLOOKUP(D62,G$2:H$15,2)</f>
+        <f t="shared" si="2"/>
         <v>staple</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lots of different updates. Should have done this sooner.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="880" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3180" yWindow="900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to make the facet graphs work.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -374,9 +374,6 @@
     <t>roots, tubers, and plantains</t>
   </si>
   <si>
-    <t>rootsNPlaintain</t>
-  </si>
-  <si>
     <t>Bovine meat</t>
   </si>
   <si>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>staple_code</t>
+  </si>
+  <si>
+    <t>rootsNPlantain</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,25 +1051,25 @@
         <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1161,7 +1161,7 @@
         <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>69</v>
@@ -1273,7 +1273,7 @@
         <v>89</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>69</v>
@@ -1301,7 +1301,7 @@
         <v>90</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>69</v>
@@ -1329,7 +1329,7 @@
         <v>88</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>69</v>
@@ -1402,7 +1402,7 @@
         <v>113</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>81</v>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>72</v>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>rootsNPlaintain</v>
+        <v>rootsNPlantain</v>
       </c>
       <c r="E22" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1602,7 +1602,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>66</v>
@@ -1678,7 +1678,7 @@
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>73</v>
@@ -1697,7 +1697,7 @@
         <v>44</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>110</v>
@@ -1716,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>72</v>
@@ -1773,7 +1773,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>64</v>
@@ -1811,7 +1811,7 @@
         <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>65</v>
@@ -1830,7 +1830,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>66</v>
@@ -1849,14 +1849,14 @@
         <v>25</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>rootsNPlaintain</v>
+        <v>rootsNPlantain</v>
       </c>
       <c r="E36" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1868,7 +1868,7 @@
         <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>110</v>
@@ -1887,7 +1887,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>66</v>
@@ -1906,7 +1906,7 @@
         <v>54</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>73</v>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>rootsNPlaintain</v>
+        <v>rootsNPlantain</v>
       </c>
       <c r="E40" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1944,7 +1944,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>73</v>
@@ -1963,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>72</v>
@@ -1982,14 +1982,14 @@
         <v>21</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>rootsNPlaintain</v>
+        <v>rootsNPlantain</v>
       </c>
       <c r="E43" s="6" t="str">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>72</v>
@@ -2020,7 +2020,7 @@
         <v>13</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>65</v>
@@ -2039,7 +2039,7 @@
         <v>48</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>73</v>
@@ -2077,7 +2077,7 @@
         <v>50</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>73</v>
@@ -2096,7 +2096,7 @@
         <v>52</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>73</v>
@@ -2115,7 +2115,7 @@
         <v>51</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>110</v>
@@ -2153,7 +2153,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>110</v>
@@ -2172,7 +2172,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>70</v>
@@ -2191,7 +2191,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>74</v>
@@ -2210,14 +2210,14 @@
         <v>22</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>rootsNPlaintain</v>
+        <v>rootsNPlantain</v>
       </c>
       <c r="E55" s="6" t="str">
         <f t="shared" si="2"/>
@@ -2248,7 +2248,7 @@
         <v>40</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>70</v>
@@ -2267,7 +2267,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>110</v>
@@ -2286,7 +2286,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
mostly changes for the facet maps. Plus some new scripts for data summarization.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="11040" yWindow="1240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
   <si>
     <t>cbeef</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>rootsNPlantain</t>
+  </si>
+  <si>
+    <t>beverages, coffee/tea/cocoa</t>
   </si>
 </sst>
 </file>
@@ -1029,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,7 +1103,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>96</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>nonstaple</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>75</v>
@@ -1571,7 +1574,7 @@
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>beverages</v>
+        <v>alcohol</v>
       </c>
       <c r="E21" s="6" t="str">
         <f t="shared" si="2"/>
@@ -1616,7 +1619,7 @@
         <v>staple</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>57</v>
       </c>
@@ -1624,11 +1627,11 @@
         <v>58</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>nutsNseeds</v>
+        <v>beverages</v>
       </c>
       <c r="E24" s="6" t="str">
         <f t="shared" si="2"/>
@@ -2236,7 +2239,7 @@
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>beverages</v>
+        <v>alcohol</v>
       </c>
       <c r="E56" s="6" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Many changes to fix annoying bugs.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10701"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/nutrientDetails/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C159C-0661-8B49-90A0-219128F41255}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="1240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8000" yWindow="1240" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$62</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="154">
   <si>
     <t>cbeef</t>
   </si>
@@ -234,9 +235,6 @@
   </si>
   <si>
     <t>eggs</t>
-  </si>
-  <si>
-    <t>roots and tubers</t>
   </si>
   <si>
     <t>fish</t>
@@ -500,7 +498,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -703,6 +701,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1029,11 +1030,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1051,39 +1052,39 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D17" si="0">VLOOKUP(C2,F$2:G$15,2)</f>
@@ -1094,24 +1095,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1122,24 +1123,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1156,18 +1157,18 @@
         <v>65</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1184,18 +1185,18 @@
         <v>64</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1212,18 +1213,18 @@
         <v>67</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1234,24 +1235,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1262,24 +1263,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1290,24 +1291,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1318,24 +1319,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1346,24 +1347,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="H11" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1380,18 +1381,18 @@
         <v>66</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1402,24 +1403,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1430,24 +1431,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1458,24 +1459,24 @@
         <v>nonstaple</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1494,7 +1495,7 @@
         <v>36</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1548,10 +1549,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1570,7 +1571,7 @@
         <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1589,7 +1590,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1605,7 +1606,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>66</v>
@@ -1627,7 +1628,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1681,10 +1682,10 @@
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1700,10 +1701,10 @@
         <v>44</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1719,10 +1720,10 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1776,7 +1777,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>64</v>
@@ -1814,7 +1815,7 @@
         <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>65</v>
@@ -1833,7 +1834,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>66</v>
@@ -1852,10 +1853,10 @@
         <v>25</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1871,10 +1872,10 @@
         <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1890,7 +1891,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>66</v>
@@ -1909,10 +1910,10 @@
         <v>54</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1931,7 +1932,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1947,10 +1948,10 @@
         <v>53</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1966,10 +1967,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1985,10 +1986,10 @@
         <v>21</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2004,10 +2005,10 @@
         <v>3</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D44" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2023,7 +2024,7 @@
         <v>13</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>65</v>
@@ -2042,10 +2043,10 @@
         <v>48</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D46" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2064,7 +2065,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2080,10 +2081,10 @@
         <v>50</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2099,10 +2100,10 @@
         <v>52</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2118,10 +2119,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2156,10 +2157,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2175,10 +2176,10 @@
         <v>39</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2194,10 +2195,10 @@
         <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D54" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2213,10 +2214,10 @@
         <v>22</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2235,7 +2236,7 @@
         <v>62</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2251,10 +2252,10 @@
         <v>40</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2270,10 +2271,10 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2289,10 +2290,10 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D59" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2311,7 +2312,7 @@
         <v>42</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D60" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2341,7 +2342,7 @@
         <v>staple</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>23</v>
       </c>
@@ -2349,11 +2350,11 @@
         <v>24</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>pulses</v>
+        <v>rootsNPlantain</v>
       </c>
       <c r="E62" s="6" t="str">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
A whole bunch of small changes.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/food commodity to food group table V4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10904"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/nutrientDetails/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C159C-0661-8B49-90A0-219128F41255}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B593340-C253-754B-9226-B2464283893C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8000" yWindow="1240" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,9 +360,6 @@
     <t>beverages, alcoholic</t>
   </si>
   <si>
-    <t>nuts and seeds</t>
-  </si>
-  <si>
     <t>nutsNseeds</t>
   </si>
   <si>
@@ -493,6 +490,9 @@
   </si>
   <si>
     <t>beverages, coffee/tea/cocoa</t>
+  </si>
+  <si>
+    <t>nuts and oilseeds</t>
   </si>
 </sst>
 </file>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1055,25 +1055,25 @@
         <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>148</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1123,7 +1123,7 @@
         <v>nonstaple</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>74</v>
@@ -1165,7 +1165,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>68</v>
@@ -1277,7 +1277,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>68</v>
@@ -1305,7 +1305,7 @@
         <v>89</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>68</v>
@@ -1328,12 +1328,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>87</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>68</v>
@@ -1347,10 +1347,10 @@
         <v>nonstaple</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>79</v>
@@ -1403,10 +1403,10 @@
         <v>nonstaple</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>80</v>
@@ -1549,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>71</v>
@@ -1571,7 +1571,7 @@
         <v>60</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1590,7 +1590,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1606,7 +1606,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>66</v>
@@ -1628,7 +1628,7 @@
         <v>58</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1682,7 +1682,7 @@
         <v>45</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>72</v>
@@ -1696,15 +1696,15 @@
         <v>nonstaple</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1720,7 +1720,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>71</v>
@@ -1777,7 +1777,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>64</v>
@@ -1815,7 +1815,7 @@
         <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>65</v>
@@ -1834,7 +1834,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>66</v>
@@ -1853,10 +1853,10 @@
         <v>25</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1867,15 +1867,15 @@
         <v>staple</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1891,7 +1891,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>66</v>
@@ -1910,7 +1910,7 @@
         <v>54</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>72</v>
@@ -1932,7 +1932,7 @@
         <v>38</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D40" s="6" t="str">
         <f t="shared" si="3"/>
@@ -1948,7 +1948,7 @@
         <v>53</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>72</v>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>71</v>
@@ -1986,10 +1986,10 @@
         <v>21</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2005,7 +2005,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>71</v>
@@ -2024,7 +2024,7 @@
         <v>13</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>65</v>
@@ -2043,7 +2043,7 @@
         <v>48</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>72</v>
@@ -2057,7 +2057,7 @@
         <v>nonstaple</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>46</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="D47" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2081,7 +2081,7 @@
         <v>50</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>72</v>
@@ -2100,7 +2100,7 @@
         <v>52</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>72</v>
@@ -2114,15 +2114,15 @@
         <v>nonstaple</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="D50" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2152,15 +2152,15 @@
         <v>staple</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="D52" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2176,7 +2176,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>69</v>
@@ -2195,7 +2195,7 @@
         <v>43</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>73</v>
@@ -2214,10 +2214,10 @@
         <v>22</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D55" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2236,7 +2236,7 @@
         <v>62</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2252,7 +2252,7 @@
         <v>40</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>69</v>
@@ -2266,15 +2266,15 @@
         <v>nonstaple</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="D58" s="6" t="str">
         <f t="shared" si="3"/>
@@ -2290,7 +2290,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>72</v>
@@ -2350,7 +2350,7 @@
         <v>24</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D62" s="6" t="str">
         <f t="shared" si="3"/>

</xml_diff>